<commit_message>
Testing of main preparation file, small adjustments in input excel files
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/diesel/Model_Data_Base_diesel.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/diesel/Model_Data_Base_diesel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/diesel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/diesel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="282" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD7F9579-AA48-4111-8FCD-B7C7EC2A82CE}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A64B7CF2-F30C-4AC1-A6FA-1570ACF195E2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-3840" yWindow="-21720" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1585,7 +1585,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1675,6 +1675,9 @@
       </c>
       <c r="D3" t="b">
         <v>1</v>
+      </c>
+      <c r="E3">
+        <v>9999</v>
       </c>
       <c r="G3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Error in methane/jet_fuel input + temporal resolution update
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Products/diesel/Model_Data_Base_diesel.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Products/diesel/Model_Data_Base_diesel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Products/diesel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B5F29A4A-EA87-4677-8B97-7434E8C6C701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57CC8033-9C36-4E07-A9DC-1916FD51FD74}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{B5F29A4A-EA87-4677-8B97-7434E8C6C701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70518CDC-0953-4002-8148-6128F0931880}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -1706,7 +1706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -2500,8 +2500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2749,6 +2749,9 @@
       </c>
       <c r="G4" t="s">
         <v>32</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.35">

</xml_diff>